<commit_message>
actual qualifier ranks | per ctr cockpit
</commit_message>
<xml_diff>
--- a/data/R_act_qualifier_cockpit.xlsx
+++ b/data/R_act_qualifier_cockpit.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diiim\Documents\job_uni\Master\Thesis\F1_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30059503-C1D8-4AD2-96FB-95A4E43E42BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFC5F4A-1F16-47CC-B4A2-EA728D775088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -499,17 +499,23 @@
     <t>V159</t>
   </si>
   <si>
-    <t>V160</t>
+    <t>V0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -836,491 +842,491 @@
   <dimension ref="A1:FD25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="FD1" sqref="FD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:160" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CP1" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CQ1" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CR1" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CS1" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CT1" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CU1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CV1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CW1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CX1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CY1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DB1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DC1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DD1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DE1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DF1" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DG1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DH1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DI1" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DJ1" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DK1" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DL1" t="s">
         <v>114</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DM1" t="s">
         <v>115</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DN1" t="s">
         <v>116</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DO1" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DP1" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DQ1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DR1" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DS1" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DT1" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DU1" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DV1" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="DW1" t="s">
         <v>125</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="DX1" t="s">
         <v>126</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="DY1" t="s">
         <v>127</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="DZ1" t="s">
         <v>128</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EA1" t="s">
         <v>129</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EB1" t="s">
         <v>130</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EC1" t="s">
         <v>131</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="ED1" t="s">
         <v>132</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EE1" t="s">
         <v>133</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EF1" t="s">
         <v>134</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EG1" t="s">
         <v>135</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EH1" t="s">
         <v>136</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EI1" t="s">
         <v>137</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EJ1" t="s">
         <v>138</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EK1" t="s">
         <v>139</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="EL1" t="s">
         <v>140</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EM1" t="s">
         <v>141</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EN1" t="s">
         <v>142</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="EO1" t="s">
         <v>143</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="EP1" t="s">
         <v>144</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="EQ1" t="s">
         <v>145</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="ER1" t="s">
         <v>146</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="ES1" t="s">
         <v>147</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="ET1" t="s">
         <v>148</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="EU1" t="s">
         <v>149</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EV1" t="s">
         <v>150</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EW1" t="s">
         <v>151</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="EX1" t="s">
         <v>152</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="EY1" t="s">
         <v>153</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="EZ1" t="s">
         <v>154</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FA1" t="s">
         <v>155</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="FB1" t="s">
         <v>156</v>
       </c>
-      <c r="FB1" t="s">
+      <c r="FC1" t="s">
         <v>157</v>
       </c>
-      <c r="FC1" t="s">
+      <c r="FD1" t="s">
         <v>158</v>
-      </c>
-      <c r="FD1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:160" x14ac:dyDescent="0.35">
@@ -11182,6 +11188,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>